<commit_message>
Update 支持 hunter 资产收集
</commit_message>
<xml_diff>
--- a/results/fofa_result.xlsx
+++ b/results/fofa_result.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Security file\chunsou\最终版本\v1.3\chunsou_正式版_version_1.3\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Security file\chunsou\最终版本\chunsou_v1.3\chunsou_github_version_1.3\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B141446-76E0-494D-BB1F-EF95CC5DFEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D79374-8970-471A-8479-CC4984552992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,20 +425,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" customWidth="1"/>
-    <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="44.44140625" customWidth="1"/>
+    <col min="1" max="1" width="49.21875" customWidth="1"/>
+    <col min="2" max="2" width="246" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="49.21875" customWidth="1"/>
     <col min="5" max="5" width="19.21875" customWidth="1"/>
     <col min="6" max="6" width="6" customWidth="1"/>
     <col min="7" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="8" width="21.5546875" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
@@ -480,6 +480,5 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>